<commit_message>
set check again 追加
</commit_message>
<xml_diff>
--- a/psggConverter/psggConverterLib/sm/SourceControl.xlsx
+++ b/psggConverter/psggConverterLib/sm/SourceControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C2AA11-4DA8-4052-A9C8-CA10AE97D217}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC9A26D-E507-47C3-AFD2-FB65DDF7660E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="139">
   <si>
     <t>thumbnail</t>
   </si>
@@ -638,14 +638,6 @@
   </si>
   <si>
     <t>br_CONTINUE(S_NEXT_LC);
-br_NOTABOVE(S_IS_MACRO_LC);</t>
-  </si>
-  <si>
-    <t>br_CONTINUE(S_NEXT_LC);
-br_NOTABOVE(S_ADDLINE_LC);</t>
-  </si>
-  <si>
-    <t>br_CONTINUE(S_NEXT_LC);
 br_NOTABOVE(S_IS_CONTENTS_1_LC);</t>
   </si>
   <si>
@@ -721,7 +713,27 @@
     <t>100027</t>
   </si>
   <si>
-    <t xml:space="preserve">; The setting was created automatically. 2018/07/25 21:48:19
+    <t>S_SET_CHECKAGAIN</t>
+  </si>
+  <si>
+    <t>再変換要素がある可能性があるので、再チェック依頼</t>
+  </si>
+  <si>
+    <t>set_check_again();</t>
+  </si>
+  <si>
+    <t>br_CONTINUE(S_SET_CHECKAGAIN);
+br_NOTABOVE(S_IS_MACRO_LC);</t>
+  </si>
+  <si>
+    <t>br_CONTINUE(S_SET_CHECKAGAIN);
+br_NOTABOVE(S_ADDLINE_LC);</t>
+  </si>
+  <si>
+    <t>100028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; The setting was created automatically. 2018/07/26 20:10:44
 ; * pssgEditor version : 0.7.0.2ad44cf1b143dddc32824edf59c45afea3d2c899
 psggfile=@@@
 SourceControl.psgg
@@ -739,7 +751,7 @@
 c_contents=1
 force_display_outpin=0
 last_action=@@@
-Changed an arrow direction
+Initilized
 @@@
 target_pathdir=@@@
 /CreateSource/LineConvert/
@@ -747,7 +759,7 @@
 state_location_list=@@@
 @@@
 fillter_state_location_list=@@@
-[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":28,"y":41}},{"Key":"S_END","Value":{"x":36.2353439,"y":553.6471}},{"Key":"S_LOADSETTING","Value":{"x":21,"y":179}},{"Key":"S_SETLANG","Value":{"x":206,"y":176}},{"Key":"S_WRITEHEDDER","Value":{"x":399,"y":181}},{"Key":"S_CREATESOURCE","Value":{"x":608,"y":185}},{"Key":"S_WRITEFILE","Value":{"x":1026.05884,"y":187.176437}},{"Key":"____altnative_state____CreateSource","Value":{"x":608,"y":185}},{"Key":"S_0001","Value":{"x":841.1765,"y":500}},{"Key":"S_ESCAPE_TO_CHAR","Value":{"x":836.470642,"y":188.23526}}]},{"Key":"\/CreateSource\/","Value":[{"Key":"S_WRITEHEDDER","Value":{"x":19,"y":16}},{"Key":"S_CREATESOURCE","Value":{"x":37.94117,"y":202.235321}},{"Key":"S_WRITEFILE","Value":{"x":889.1764,"y":391.117676}},{"Key":"S_CONTENTS_2","Value":{"x":396.529419,"y":375.529419}},{"Key":"S_CONTENTS_1","Value":{"x":185.823532,"y":373.176483}},{"Key":"S_SETUP_LINECONVERT","Value":{"x":63,"y":400}},{"Key":"S_CHECKCOUNT_LINECONVERT","Value":{"x":277,"y":403}},{"Key":"____altnative_state____LineConvert","Value":{"x":635,"y":382}},{"Key":"S_ESCAPE_TO_CHAR","Value":{"x":927.941162,"y":314.352966}}]},{"Key":"\/CreateSource\/LineConvert\/","Value":[{"Key":"S_CONTENTS_2","Value":{"x":45,"y":27}},{"Key":"S_SETUP_LINECONVERT","Value":{"x":40,"y":183}},{"Key":"S_CHECKCOUNT_LINECONVERT","Value":{"x":235,"y":184}},{"Key":"S_WRITEFILE","Value":{"x":1068.88232,"y":241.9412}},{"Key":"S_GETLINE_LINECONVERT","Value":{"x":39,"y":611}},{"Key":"S_IS_END_LINECONVERT","Value":{"x":239,"y":609}},{"Key":"S_IS_CONTENTS_1_LINECONVERT","Value":{"x":468,"y":603}},{"Key":"S_IS_CONTENTS_1_LINECONVERT1","Value":{"x":702,"y":596}},{"Key":"S_IS_INCLUDE_LINECONVERT","Value":{"x":920,"y":606}},{"Key":"S_IS_MACRO_LINECONVERT1","Value":{"x":1123,"y":603}},{"Key":"S_NEXT_LINECONVERT","Value":{"x":1387,"y":288}},{"Key":"S_ADDLINE_LINECONVERT","Value":{"x":1376.52942,"y":662.7059}},{"Key":"S_SETUP_LC","Value":{"x":42.3529358,"y":211.235291}},{"Key":"S_CHECKCOUNT_LC","Value":{"x":444.4118,"y":204.000015}},{"Key":"S_GETLINE_LC","Value":{"x":31.94117,"y":436.882355}},{"Key":"S_IS_END_LC","Value":{"x":215.470581,"y":519.588257}},{"Key":"S_IS_CONTENTS_1_LC","Value":{"x":657.235352,"y":755.647156}},{"Key":"S_IS_CONTENTS_2_LC","Value":{"x":893.588135,"y":875.706}},{"Key":"S_IS_INCLUDE_LC","Value":{"x":1175.11743,"y":863.353}},{"Key":"S_IS_MACRO_LC","Value":{"x":1445.17664,"y":880.352966}},{"Key":"S_ADDLINE_LC","Value":{"x":1723.41174,"y":810.6471}},{"Key":"S_NEXT_LC","Value":{"x":1387,"y":288}},{"Key":"S_0001","Value":{"x":1103.52942,"y":208.2353}},{"Key":"S_CHECK_AGAIN","Value":{"x":867.059,"y":214.117737}},{"Key":"S_SETUP2_LC","Value":{"x":234.117676,"y":210.588272}},{"Key":"S_IS_COMMENT","Value":{"x":428.235321,"y":642.353}},{"Key":"S_ESCAPE_TO_CHAR","Value":{"x":1362.00012,"y":89.41182}},{"Key":"S_LINESTOBUF_LC","Value":{"x":660.000061,"y":216.4706}},{"Key":"S_BIND_SRC","Value":{"x":1103.52942,"y":208.2353}}]}]
+[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":28,"y":41}},{"Key":"S_END","Value":{"x":36.2353439,"y":553.6471}},{"Key":"S_LOADSETTING","Value":{"x":21,"y":179}},{"Key":"S_SETLANG","Value":{"x":206,"y":176}},{"Key":"S_WRITEHEDDER","Value":{"x":399,"y":181}},{"Key":"S_CREATESOURCE","Value":{"x":608,"y":185}},{"Key":"S_WRITEFILE","Value":{"x":1026.05884,"y":187.176437}},{"Key":"S_ESCAPE_TO_CHAR","Value":{"x":836.470642,"y":188.23526}}]},{"Key":"\/CreateSource\/","Value":[{"Key":"S_WRITEHEDDER","Value":{"x":19,"y":16}},{"Key":"S_CREATESOURCE","Value":{"x":37.94117,"y":202.235321}},{"Key":"S_WRITEFILE","Value":{"x":889.1764,"y":391.117676}},{"Key":"S_CONTENTS_2","Value":{"x":396.529419,"y":375.529419}},{"Key":"S_CONTENTS_1","Value":{"x":185.823532,"y":373.176483}},{"Key":"S_ESCAPE_TO_CHAR","Value":{"x":927.941162,"y":314.352966}}]},{"Key":"\/CreateSource\/LineConvert\/","Value":[{"Key":"S_CONTENTS_2","Value":{"x":45,"y":27}},{"Key":"S_WRITEFILE","Value":{"x":1068.88232,"y":241.9412}},{"Key":"S_SETUP_LC","Value":{"x":42.3529358,"y":211.235291}},{"Key":"S_CHECKCOUNT_LC","Value":{"x":444.4118,"y":204.000015}},{"Key":"S_GETLINE_LC","Value":{"x":31.94117,"y":436.882355}},{"Key":"S_IS_END_LC","Value":{"x":215.470581,"y":519.588257}},{"Key":"S_IS_CONTENTS_1_LC","Value":{"x":657.235352,"y":755.647156}},{"Key":"S_IS_CONTENTS_2_LC","Value":{"x":893.588135,"y":875.706}},{"Key":"S_IS_INCLUDE_LC","Value":{"x":1175.11743,"y":863.353}},{"Key":"S_IS_MACRO_LC","Value":{"x":1445.17664,"y":880.352966}},{"Key":"S_ADDLINE_LC","Value":{"x":1723.41174,"y":810.6471}},{"Key":"S_NEXT_LC","Value":{"x":1598,"y":229}},{"Key":"S_CHECK_AGAIN","Value":{"x":867.059,"y":214.117737}},{"Key":"S_SETUP2_LC","Value":{"x":234.117676,"y":210.588272}},{"Key":"S_IS_COMMENT","Value":{"x":428.235321,"y":642.353}},{"Key":"S_ESCAPE_TO_CHAR","Value":{"x":1362.00012,"y":89.41182}},{"Key":"S_LINESTOBUF_LC","Value":{"x":660.000061,"y":216.4706}},{"Key":"S_BIND_SRC","Value":{"x":1103.52942,"y":208.2353}},{"Key":"S_SET_CHECKAGAIN","Value":{"x":1395,"y":589}}]}]
 @@@
 linecolor_data=@@@
 [{"color":{"knownColor":0,"name":null,"state":2,"value":4282417280},"pattern":"br_CONTINUE"}]
@@ -1407,6 +1419,9 @@
       <c r="AA1" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="AB1" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="AC1" s="2" t="s">
         <v>29</v>
       </c>
@@ -1480,16 +1495,19 @@
         <v>102</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="AC2" s="4" t="s">
         <v>98</v>
@@ -1560,16 +1578,19 @@
         <v>103</v>
       </c>
       <c r="X3" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Y3" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Z3" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AA3" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
+      </c>
+      <c r="AB3" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="AC3" s="7" t="s">
         <v>99</v>
@@ -1639,7 +1660,10 @@
         <v>34</v>
       </c>
       <c r="AA5" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="AB5" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:29" s="11" customFormat="1">
@@ -1694,7 +1718,7 @@
         <v>92</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S7" s="11" t="s">
         <v>93</v>
@@ -1712,19 +1736,22 @@
         <v>105</v>
       </c>
       <c r="X7" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Z7" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AA7" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
+      </c>
+      <c r="AB7" s="11" t="s">
+        <v>134</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:29" s="11" customFormat="1" ht="37.5">
@@ -1830,7 +1857,7 @@
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:29" s="13" customFormat="1" ht="93.75">
+    <row r="20" spans="1:29" s="13" customFormat="1" ht="112.5">
       <c r="A20" s="12"/>
       <c r="B20" s="12" t="s">
         <v>23</v>
@@ -1839,7 +1866,7 @@
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="O20" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P20" s="13" t="s">
         <v>107</v>
@@ -1848,19 +1875,19 @@
         <v>108</v>
       </c>
       <c r="R20" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="S20" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="V20" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="X20" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="S20" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="V20" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="X20" s="13" t="s">
-        <v>111</v>
-      </c>
       <c r="AC20" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:29" s="15" customFormat="1" ht="18.75" customHeight="1">
@@ -1941,13 +1968,16 @@
         <v>97</v>
       </c>
       <c r="Y23" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Z23" s="16" t="s">
         <v>57</v>
       </c>
       <c r="AA23" s="16" t="s">
-        <v>127</v>
+        <v>125</v>
+      </c>
+      <c r="AB23" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="AC23" s="16" t="s">
         <v>97</v>
@@ -2018,16 +2048,19 @@
         <v>106</v>
       </c>
       <c r="X24" s="16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Y24" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Z24" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AA24" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
+      </c>
+      <c r="AB24" s="16" t="s">
+        <v>137</v>
       </c>
       <c r="AC24" s="16" t="s">
         <v>100</v>
@@ -2050,7 +2083,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="409.5">
       <c r="A1" s="18" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>